<commit_message>
ART-791: test cases described in Artisan 2 - Updating Methodology - Excel Demo - v103.xls added. All worked fine. No corrections in code required.
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/AggregateBFUpdateAtStart.xlsx
+++ b/test/data/spreadsheets/AggregateBFUpdateAtStart.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="360" yWindow="375" windowWidth="18795" windowHeight="11505"/>
   </bookViews>
   <sheets>
-    <sheet name="Usage" sheetId="3" r:id="rId1"/>
+    <sheet name="Usage" sheetId="8" r:id="rId1"/>
     <sheet name="Pattern" sheetId="6" r:id="rId2"/>
     <sheet name="Claims" sheetId="5" r:id="rId3"/>
     <sheet name="Results" sheetId="7" r:id="rId4"/>
@@ -37,10 +37,12 @@
     <definedName name="RiskBeforeRecalcMacro" hidden="1">""</definedName>
     <definedName name="RiskBeforeSimMacro" hidden="1">""</definedName>
     <definedName name="RiskCollectDistributionSamples" hidden="1">0</definedName>
+    <definedName name="RiskFixedSeed" localSheetId="0" hidden="1">1</definedName>
     <definedName name="RiskFixedSeed" hidden="1">123</definedName>
     <definedName name="RiskHasSettings" hidden="1">5</definedName>
     <definedName name="RiskMinimizeOnStart" hidden="1">FALSE</definedName>
     <definedName name="RiskMonitorConvergence" hidden="1">TRUE</definedName>
+    <definedName name="RiskNumIterations" localSheetId="0" hidden="1">1000</definedName>
     <definedName name="RiskNumIterations" hidden="1">500</definedName>
     <definedName name="RiskNumSimulations" hidden="1">1</definedName>
     <definedName name="RiskPauseOnError" hidden="1">FALSE</definedName>
@@ -52,6 +54,7 @@
     <definedName name="RiskStandardRecalc" hidden="1">2</definedName>
     <definedName name="RiskUpdateDisplay" hidden="1">FALSE</definedName>
     <definedName name="RiskUseDifferentSeedForEachSim" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseFixedSeed" localSheetId="0" hidden="1">FALSE</definedName>
     <definedName name="RiskUseFixedSeed" hidden="1">TRUE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">FALSE</definedName>
   </definedNames>
@@ -59,42 +62,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>sku</author>
-  </authors>
-  <commentList>
-    <comment ref="E34" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>sku:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Chris will provide a corrected spreadsheet</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>1) Inputs</t>
   </si>
@@ -214,6 +183,12 @@
   </si>
   <si>
     <t>Adjusted Ultimate</t>
+  </si>
+  <si>
+    <t>Get most recent reported on or before the update date</t>
+  </si>
+  <si>
+    <t>Note: If pattern has "run out" default to 100</t>
   </si>
 </sst>
 </file>
@@ -230,7 +205,7 @@
     <numFmt numFmtId="170" formatCode="#,##0.00;\(#,##0.00\);\-"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,27 +267,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,8 +287,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -420,13 +382,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -558,10 +557,16 @@
     <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="7" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Dezimal" xfId="1" builtinId="3"/>
@@ -858,10 +863,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="3" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="D2:AA126"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -984,6 +992,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="23">
+        <f>E9</f>
         <v>40179</v>
       </c>
       <c r="F12" s="30"/>
@@ -1113,7 +1122,7 @@
         <v>45000</v>
       </c>
       <c r="H19" s="23">
-        <v>40998</v>
+        <v>40908</v>
       </c>
       <c r="I19" s="23"/>
       <c r="K19" s="30"/>
@@ -1152,7 +1161,7 @@
         <v>25000</v>
       </c>
       <c r="H20" s="23">
-        <v>40998</v>
+        <v>40908</v>
       </c>
       <c r="I20" s="23"/>
       <c r="K20" s="30"/>
@@ -1192,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="23">
-        <v>40998</v>
+        <v>40908</v>
       </c>
       <c r="I21" s="23"/>
       <c r="K21" s="30"/>
@@ -1210,10 +1219,18 @@
     </row>
     <row r="22" spans="4:27">
       <c r="D22" s="29"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
+      <c r="E22" s="34">
+        <v>1</v>
+      </c>
+      <c r="F22" s="34">
+        <v>75000</v>
+      </c>
+      <c r="G22" s="34">
+        <v>55000</v>
+      </c>
+      <c r="H22" s="23">
+        <v>40998</v>
+      </c>
       <c r="I22" s="23"/>
       <c r="K22" s="30"/>
       <c r="L22" s="41">
@@ -1230,10 +1247,18 @@
     </row>
     <row r="23" spans="4:27">
       <c r="D23" s="29"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
+      <c r="E23" s="34">
+        <v>2</v>
+      </c>
+      <c r="F23" s="34">
+        <v>50000</v>
+      </c>
+      <c r="G23" s="34">
+        <v>32000</v>
+      </c>
+      <c r="H23" s="23">
+        <v>40998</v>
+      </c>
       <c r="I23" s="44"/>
       <c r="K23" s="30"/>
       <c r="L23" s="41"/>
@@ -1245,10 +1270,18 @@
     </row>
     <row r="24" spans="4:27">
       <c r="D24" s="29"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
+      <c r="E24" s="34">
+        <v>3</v>
+      </c>
+      <c r="F24" s="34">
+        <v>10000</v>
+      </c>
+      <c r="G24" s="34">
+        <v>10000</v>
+      </c>
+      <c r="H24" s="23">
+        <v>40998</v>
+      </c>
       <c r="I24" s="44"/>
       <c r="K24" s="30"/>
       <c r="L24" s="41"/>
@@ -1347,7 +1380,7 @@
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="4:9">
+    <row r="33" spans="4:9" ht="15.75" thickBot="1">
       <c r="D33" s="3" t="s">
         <v>2</v>
       </c>
@@ -1363,9 +1396,9 @@
       <c r="D34" s="3">
         <v>1</v>
       </c>
-      <c r="E34" s="57">
+      <c r="E34" s="58">
         <f ca="1">$F$58</f>
-        <v>125000</v>
+        <v>75000</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
@@ -1376,22 +1409,22 @@
       <c r="D35" s="3">
         <v>2</v>
       </c>
-      <c r="E35" s="57">
+      <c r="E35" s="59">
         <f ca="1">$G$58</f>
-        <v>117500</v>
+        <v>75000</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="4:9">
+    <row r="36" spans="4:9" ht="15.75" thickBot="1">
       <c r="D36" s="3">
         <v>3</v>
       </c>
-      <c r="E36" s="57">
+      <c r="E36" s="60">
         <f ca="1">$H$58</f>
-        <v>82500</v>
+        <v>75000</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="20"/>
@@ -1418,7 +1451,7 @@
         <v>11</v>
       </c>
       <c r="F40" s="9">
-        <f t="array" ref="F40">MAX(IF($H$19:$H$28&lt;$E$12,$H$19:$H$28))</f>
+        <f t="array" ref="F40">MAX(IF($H$19:$H$28&lt;=$E$12,$H$19:$H$28))</f>
         <v>0</v>
       </c>
       <c r="G40" s="49" t="s">
@@ -1464,15 +1497,15 @@
         <v>12</v>
       </c>
       <c r="F44" s="10">
-        <f>IF($F$40=0,0,DAYS360(F$43,$F$40)/30)</f>
+        <f>IF(OR($F$40=0,F$43&gt;=$E$12),0,DAYS360(F$43,$F$40)/30)</f>
         <v>0</v>
       </c>
       <c r="G44" s="10">
-        <f>IF($F$40=0,0,DAYS360(G$43,$F$40)/30)</f>
+        <f>IF(OR($F$40=0,G$43&gt;=$E$12),0,DAYS360(G$43,$F$40)/30)</f>
         <v>0</v>
       </c>
       <c r="H44" s="10">
-        <f>IF($F$40=0,0,DAYS360(H$43,$F$40)/30)</f>
+        <f>IF(OR($F$40=0,H$43&gt;=$E$12),0,DAYS360(H$43,$F$40)/30)</f>
         <v>0</v>
       </c>
       <c r="I44" s="49" t="s">
@@ -1484,18 +1517,20 @@
         <v>35</v>
       </c>
       <c r="F45" s="55">
-        <f>$F$19</f>
-        <v>50000</v>
+        <f>SUMIFS($F$19:$F$28,$H$19:$H$28,$F$40,$E$19:$E$28,F$42)</f>
+        <v>0</v>
       </c>
       <c r="G45" s="55">
-        <f>$F$20</f>
-        <v>42500</v>
+        <f>SUMIFS($F$19:$F$28,$H$19:$H$28,$F$40,$E$19:$E$28,G$42)</f>
+        <v>0</v>
       </c>
       <c r="H45" s="55">
-        <f>$F$21</f>
-        <v>7500</v>
-      </c>
-      <c r="I45" s="49"/>
+        <f>SUMIFS($F$19:$F$28,$H$19:$H$28,$F$40,$E$19:$E$28,H$42)</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="49" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="46" spans="4:9">
       <c r="E46" s="3"/>
@@ -1527,16 +1562,19 @@
         <v>22</v>
       </c>
       <c r="F49" s="11">
-        <f ca="1">OFFSET($M$18,F$47,0)</f>
+        <f ca="1">IF(F$47&gt;=COUNTA($M$18:$M$27),1,OFFSET($M$18,F$47,0))</f>
         <v>0.65</v>
       </c>
       <c r="G49" s="11">
-        <f ca="1">OFFSET($M$18,G$47,0)</f>
+        <f ca="1">IF(G$47&gt;=COUNTA($M$18:$M$27),1,OFFSET($M$18,G$47,0))</f>
         <v>0.65</v>
       </c>
       <c r="H49" s="11">
-        <f ca="1">OFFSET($M$18,H$47,0)</f>
+        <f ca="1">IF(H$47&gt;=COUNTA($M$18:$M$27),1,OFFSET($M$18,H$47,0))</f>
         <v>0.65</v>
+      </c>
+      <c r="I49" s="49" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="5:9">
@@ -1645,15 +1683,15 @@
       </c>
       <c r="F58" s="55">
         <f ca="1">F45+F56*$I$10</f>
-        <v>125000</v>
+        <v>75000</v>
       </c>
       <c r="G58" s="55">
         <f ca="1">G45+G56*$I$10</f>
-        <v>117500</v>
+        <v>75000</v>
       </c>
       <c r="H58" s="55">
         <f ca="1">H45+H56*$I$10</f>
-        <v>82500</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="59" spans="5:9">
@@ -1971,7 +2009,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2043,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A8" sqref="A8:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2067,43 +2104,109 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="34">
+        <f>Usage!E19</f>
         <v>1</v>
       </c>
       <c r="B2" s="34">
+        <f>Usage!F19</f>
         <v>50000</v>
       </c>
       <c r="C2" s="34">
+        <f>Usage!G19</f>
         <v>45000</v>
       </c>
       <c r="D2" s="23">
-        <v>40998</v>
+        <f>Usage!H19</f>
+        <v>40908</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="34">
+        <f>Usage!E20</f>
         <v>2</v>
       </c>
       <c r="B3" s="34">
+        <f>Usage!F20</f>
         <v>42500</v>
       </c>
       <c r="C3" s="34">
+        <f>Usage!G20</f>
         <v>25000</v>
       </c>
       <c r="D3" s="23">
-        <v>40998</v>
+        <f>Usage!H20</f>
+        <v>40908</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="34">
+        <f>Usage!E21</f>
         <v>3</v>
       </c>
       <c r="B4" s="34">
+        <f>Usage!F21</f>
         <v>7500</v>
       </c>
       <c r="C4" s="34">
+        <f>Usage!G21</f>
         <v>0</v>
       </c>
       <c r="D4" s="23">
+        <f>Usage!H21</f>
+        <v>40908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="34">
+        <f>Usage!E22</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="34">
+        <f>Usage!F22</f>
+        <v>75000</v>
+      </c>
+      <c r="C5" s="34">
+        <f>Usage!G22</f>
+        <v>55000</v>
+      </c>
+      <c r="D5" s="23">
+        <f>Usage!H22</f>
+        <v>40998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="34">
+        <f>Usage!E23</f>
+        <v>2</v>
+      </c>
+      <c r="B6" s="34">
+        <f>Usage!F23</f>
+        <v>50000</v>
+      </c>
+      <c r="C6" s="34">
+        <f>Usage!G23</f>
+        <v>32000</v>
+      </c>
+      <c r="D6" s="23">
+        <f>Usage!H23</f>
+        <v>40998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="34">
+        <f>Usage!E24</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="34">
+        <f>Usage!F24</f>
+        <v>10000</v>
+      </c>
+      <c r="C7" s="34">
+        <f>Usage!G24</f>
+        <v>10000</v>
+      </c>
+      <c r="D7" s="23">
+        <f>Usage!H24</f>
         <v>40998</v>
       </c>
     </row>
@@ -2131,17 +2234,17 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="58">
+      <c r="A2" s="57">
         <v>75000</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="58">
+      <c r="A3" s="57">
         <v>75000</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="58">
+      <c r="A4" s="57">
         <v>75000</v>
       </c>
     </row>

</xml_diff>